<commit_message>
03/27/22, almost done with auto email for manifest email to a prison, need to just convert xlsx to PDF before attaching to email.
</commit_message>
<xml_diff>
--- a/Manifest-EmailTemplate.xlsx
+++ b/Manifest-EmailTemplate.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Email:</t>
   </si>
   <si>
-    <t xml:space="preserve">Manifest Reference #</t>
+    <t xml:space="preserve">Manifest Ref #</t>
   </si>
   <si>
     <t xml:space="preserve">Name and Inmate #</t>
@@ -47,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -72,6 +72,19 @@
     <font>
       <b val="true"/>
       <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -154,7 +167,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,35 +184,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,13 +311,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>187920</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>777960</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>242280</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -301,8 +326,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="0" y="2177280"/>
-          <a:ext cx="5606280" cy="3600"/>
+          <a:off x="0" y="2213280"/>
+          <a:ext cx="5606640" cy="3600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -327,14 +352,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>774000</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:colOff>238320</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -343,8 +368,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2332440"/>
-          <a:ext cx="5602320" cy="2160"/>
+          <a:off x="0" y="2044440"/>
+          <a:ext cx="5602680" cy="2160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -369,14 +394,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>4680</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>785880</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>250200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -385,8 +410,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3322440"/>
-          <a:ext cx="5614200" cy="1800"/>
+          <a:off x="0" y="3538440"/>
+          <a:ext cx="5614560" cy="1800"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -417,13 +442,13 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.48"/>
@@ -435,79 +460,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="A4" s="6"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="0"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="0"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="F7" s="4"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="10"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
-      <c r="C11" s="11"/>
+      <c r="C10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="88.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12"/>
+      <c r="A12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12"/>
+      <c r="A13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12"/>
+      <c r="A14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
+      <c r="A15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
+      <c r="A17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
+      <c r="A18" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>